<commit_message>
dropout layer and filling empty rows
</commit_message>
<xml_diff>
--- a/datasets/training/sensor_dist_adj.xlsx
+++ b/datasets/training/sensor_dist_adj.xlsx
@@ -386,7 +386,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.1839907791668135</v>
+        <v>0.1839907791668134</v>
       </c>
       <c r="D2">
         <v>0.7883902402727958</v>
@@ -415,7 +415,7 @@
         <v>0.3472097349446793</v>
       </c>
       <c r="B3">
-        <v>0.1839907791668135</v>
+        <v>0.1839907791668134</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -503,7 +503,7 @@
         <v>0.6776626702836241</v>
       </c>
       <c r="J5">
-        <v>0.2145735406992289</v>
+        <v>0.2145735406992288</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -529,7 +529,7 @@
         <v>0.7204480724123816</v>
       </c>
       <c r="H6">
-        <v>0.4773670536824245</v>
+        <v>0.4773670536824244</v>
       </c>
       <c r="I6">
         <v>0.6954974985622417</v>
@@ -564,7 +564,7 @@
         <v>0.3265782868030284</v>
       </c>
       <c r="I7">
-        <v>0.8178542952919762</v>
+        <v>0.8178542953205142</v>
       </c>
       <c r="J7">
         <v>0.6500537318965819</v>
@@ -587,7 +587,7 @@
         <v>0.03396331390186405</v>
       </c>
       <c r="F8">
-        <v>0.4773670536824245</v>
+        <v>0.4773670536824244</v>
       </c>
       <c r="G8">
         <v>0.3265782868030284</v>
@@ -622,7 +622,7 @@
         <v>0.6954974985622417</v>
       </c>
       <c r="G9">
-        <v>0.8178542952919762</v>
+        <v>0.8178542953205142</v>
       </c>
       <c r="H9">
         <v>0.2054764288519491</v>
@@ -648,7 +648,7 @@
         <v>0.4665084657132775</v>
       </c>
       <c r="E10">
-        <v>0.2145735406992289</v>
+        <v>0.2145735406992288</v>
       </c>
       <c r="F10">
         <v>0.6246196902666028</v>

</xml_diff>